<commit_message>
New Contact Formular added
</commit_message>
<xml_diff>
--- a/Zeiterfassung.xlsx
+++ b/Zeiterfassung.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
   <si>
     <t>Zeiterfassung</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>GUI - Bugfixes</t>
+  </si>
+  <si>
+    <t>GUI - New Contact</t>
   </si>
 </sst>
 </file>
@@ -554,7 +557,7 @@
   <dimension ref="A1:E164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -595,7 +598,7 @@
       </c>
       <c r="C4" s="13">
         <f>SUMIF(B8:B103,"Teresa",D8:D103)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="3"/>
@@ -847,10 +850,18 @@
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="5"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="2"/>
+      <c r="A22" s="5">
+        <v>41772</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="2">
+        <v>1</v>
+      </c>
       <c r="E22" s="1"/>
     </row>
     <row r="23" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
New Contact ViewModel edited
</commit_message>
<xml_diff>
--- a/Zeiterfassung.xlsx
+++ b/Zeiterfassung.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
   <si>
     <t>Zeiterfassung</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>GUI - New Contact</t>
+  </si>
+  <si>
+    <t>GUI - Proxy - New Contact</t>
   </si>
 </sst>
 </file>
@@ -557,7 +560,7 @@
   <dimension ref="A1:E164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -598,7 +601,7 @@
       </c>
       <c r="C4" s="13">
         <f>SUMIF(B8:B103,"Teresa",D8:D103)</f>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="3"/>
@@ -880,10 +883,18 @@
       <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="5"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="2"/>
+      <c r="A24" s="5">
+        <v>41774</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="2">
+        <v>1</v>
+      </c>
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Edit Firma, Search Firma ~ radiobuttons yay
</commit_message>
<xml_diff>
--- a/Zeiterfassung.xlsx
+++ b/Zeiterfassung.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
   <si>
     <t>Zeiterfassung</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>GUI - Search Invoices, New Contact</t>
+  </si>
+  <si>
+    <t>GUI - Search Firm, Edit Firm</t>
   </si>
 </sst>
 </file>
@@ -568,8 +571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -610,7 +613,7 @@
       </c>
       <c r="C4" s="13">
         <f>SUMIF(B8:B103,"Teresa",D8:D103)</f>
-        <v>33.5</v>
+        <v>36.5</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="3"/>
@@ -938,7 +941,7 @@
     </row>
     <row r="27" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
-        <v>41764</v>
+        <v>41795</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>5</v>
@@ -952,10 +955,18 @@
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="5"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="2"/>
+      <c r="A28" s="5">
+        <v>41797</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" s="2">
+        <v>3</v>
+      </c>
       <c r="E28" s="1"/>
     </row>
     <row r="29" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Bugfixes - Edit Firm sollt nun gehn
</commit_message>
<xml_diff>
--- a/Zeiterfassung.xlsx
+++ b/Zeiterfassung.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FH\4.Semester\Software Engineering\MicroERP_Client\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teresa\Documents\Visual Studio 2013\Projects\MicroERP_Client\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="35">
   <si>
     <t>Zeiterfassung</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>Server - Contacts, Invoices, Firm überarbeitet, hinzugefügt</t>
+  </si>
+  <si>
+    <t>GUI - Bugs, Edit Firm</t>
   </si>
 </sst>
 </file>
@@ -587,7 +590,7 @@
   <dimension ref="A1:E167"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -628,7 +631,7 @@
       </c>
       <c r="C4" s="13">
         <f>SUMIF(B8:B106,"Teresa",D8:D106)</f>
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="3"/>
@@ -1075,10 +1078,18 @@
       <c r="E34" s="1"/>
     </row>
     <row r="35" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="5"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="2"/>
+      <c r="A35" s="5">
+        <v>41800</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35" s="2">
+        <v>6</v>
+      </c>
       <c r="E35" s="1"/>
     </row>
     <row r="36" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>